<commit_message>
IR Data and IR Test Code
</commit_message>
<xml_diff>
--- a/Matthew Data/Data.xlsx
+++ b/Matthew Data/Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew/Dropbox/Matthew/Documents/RBE 2002/RBE_2002-Team_10/Matthew Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC65085-2208-B746-A124-B0EA634502D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4903A9-A6BE-554B-85E0-046B677B83D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{33445F39-0564-DD43-A5BA-E2820B270D67}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{33445F39-0564-DD43-A5BA-E2820B270D67}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ultrasonic" sheetId="1" r:id="rId1"/>
+    <sheet name="IR" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>10 cm</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>Standard Dev</t>
+  </si>
+  <si>
+    <t>Voltage</t>
   </si>
 </sst>
 </file>
@@ -96,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6286D92-3237-AA46-91E0-694698445CC9}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,4 +912,500 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FA1115-8D26-4D43-97D4-9C6B9DBBD880}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C2">
+        <v>1.19</v>
+      </c>
+      <c r="D2">
+        <v>0.84</v>
+      </c>
+      <c r="E2">
+        <v>0.64</v>
+      </c>
+      <c r="F2">
+        <v>0.62</v>
+      </c>
+      <c r="G2">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>2.23</v>
+      </c>
+      <c r="C3">
+        <v>1.19</v>
+      </c>
+      <c r="D3">
+        <v>0.82</v>
+      </c>
+      <c r="E3">
+        <v>0.65</v>
+      </c>
+      <c r="F3">
+        <v>0.62</v>
+      </c>
+      <c r="G3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C4">
+        <v>1.21</v>
+      </c>
+      <c r="D4">
+        <v>0.82</v>
+      </c>
+      <c r="E4">
+        <v>0.65</v>
+      </c>
+      <c r="F4">
+        <v>0.62</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C5">
+        <v>1.21</v>
+      </c>
+      <c r="D5">
+        <v>0.82</v>
+      </c>
+      <c r="E5">
+        <v>0.65</v>
+      </c>
+      <c r="F5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G5">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C6">
+        <v>1.21</v>
+      </c>
+      <c r="D6">
+        <v>0.82</v>
+      </c>
+      <c r="E6">
+        <v>0.65</v>
+      </c>
+      <c r="F6">
+        <v>0.62</v>
+      </c>
+      <c r="G6">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>2.23</v>
+      </c>
+      <c r="C7">
+        <v>1.2</v>
+      </c>
+      <c r="D7">
+        <v>0.82</v>
+      </c>
+      <c r="E7">
+        <v>0.65</v>
+      </c>
+      <c r="F7">
+        <v>0.65</v>
+      </c>
+      <c r="G7">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C8">
+        <v>1.21</v>
+      </c>
+      <c r="D8">
+        <v>0.82</v>
+      </c>
+      <c r="E8">
+        <v>0.65</v>
+      </c>
+      <c r="F8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C9">
+        <v>1.21</v>
+      </c>
+      <c r="D9">
+        <v>0.82</v>
+      </c>
+      <c r="E9">
+        <v>0.65</v>
+      </c>
+      <c r="F9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G9">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C10">
+        <v>1.21</v>
+      </c>
+      <c r="D10">
+        <v>0.82</v>
+      </c>
+      <c r="E10">
+        <v>0.66</v>
+      </c>
+      <c r="F10">
+        <v>0.6</v>
+      </c>
+      <c r="G10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>2.23</v>
+      </c>
+      <c r="C11">
+        <v>1.21</v>
+      </c>
+      <c r="D11">
+        <v>0.82</v>
+      </c>
+      <c r="E11">
+        <v>0.65</v>
+      </c>
+      <c r="F11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G11">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>2.23</v>
+      </c>
+      <c r="C12">
+        <v>1.21</v>
+      </c>
+      <c r="D12">
+        <v>0.82</v>
+      </c>
+      <c r="E12">
+        <v>0.65</v>
+      </c>
+      <c r="F12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C13">
+        <v>1.21</v>
+      </c>
+      <c r="D13">
+        <v>0.82</v>
+      </c>
+      <c r="E13">
+        <v>0.63</v>
+      </c>
+      <c r="F13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>2.23</v>
+      </c>
+      <c r="C14">
+        <v>1.21</v>
+      </c>
+      <c r="D14">
+        <v>0.82</v>
+      </c>
+      <c r="E14">
+        <v>0.65</v>
+      </c>
+      <c r="F14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>2.23</v>
+      </c>
+      <c r="C15">
+        <v>1.21</v>
+      </c>
+      <c r="D15">
+        <v>0.82</v>
+      </c>
+      <c r="E15">
+        <v>0.65</v>
+      </c>
+      <c r="F15">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>2.23</v>
+      </c>
+      <c r="C16">
+        <v>1.21</v>
+      </c>
+      <c r="D16">
+        <v>0.82</v>
+      </c>
+      <c r="E16">
+        <v>0.65</v>
+      </c>
+      <c r="F16">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G16">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>2.23</v>
+      </c>
+      <c r="C17">
+        <v>1.21</v>
+      </c>
+      <c r="D17">
+        <v>0.82</v>
+      </c>
+      <c r="E17">
+        <v>0.65</v>
+      </c>
+      <c r="F17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>2.23</v>
+      </c>
+      <c r="C18">
+        <v>1.21</v>
+      </c>
+      <c r="D18">
+        <v>0.82</v>
+      </c>
+      <c r="E18">
+        <v>0.66</v>
+      </c>
+      <c r="F18">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>2.23</v>
+      </c>
+      <c r="C19">
+        <v>1.21</v>
+      </c>
+      <c r="D19">
+        <v>0.82</v>
+      </c>
+      <c r="E19">
+        <v>0.66</v>
+      </c>
+      <c r="F19">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G19">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2.23</v>
+      </c>
+      <c r="C20">
+        <v>1.21</v>
+      </c>
+      <c r="D20">
+        <v>0.83</v>
+      </c>
+      <c r="E20">
+        <v>0.65</v>
+      </c>
+      <c r="F20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G20">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>2.23</v>
+      </c>
+      <c r="C21">
+        <v>1.21</v>
+      </c>
+      <c r="D21">
+        <v>0.82</v>
+      </c>
+      <c r="E21">
+        <v>0.65</v>
+      </c>
+      <c r="F21">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G21">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f>AVERAGE(B2:B21)</f>
+        <v>2.2259999999999991</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:G23" si="0">AVERAGE(C2:C21)</f>
+        <v>1.2075000000000005</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.82150000000000012</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="F23">
+        <f>AVERAGE(F2:F21)</f>
+        <v>0.59150000000000003</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0.6034999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <f>STDEV(B2:B21)</f>
+        <v>5.0262468995002372E-3</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:G24" si="1">STDEV(C2:C21)</f>
+        <v>6.3866637365850541E-3</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>4.8936048492959341E-3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>6.4888568452305074E-3</v>
+      </c>
+      <c r="F24">
+        <f>STDEV(F2:F21)</f>
+        <v>2.2070461326349652E-2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1.8994459025837265E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>